<commit_message>
Updates up to page 8 in Practice 1
Tested logins
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabrielle.marhue\Documents\UiPath\ReFrameWork-UiDemo\Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="4080" windowHeight="6945"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="4080" windowHeight="6945" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -173,16 +168,19 @@
     <t>UiDemoCredential</t>
   </si>
   <si>
-    <t>UiDemoCredential_REFramework</t>
-  </si>
-  <si>
     <t>Credential used to log in to UiDemo</t>
+  </si>
+  <si>
+    <t>PasswordUID</t>
+  </si>
+  <si>
+    <t>UiDemoPath</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -279,7 +277,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -314,7 +312,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -491,7 +489,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -501,8 +499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -563,10 +561,10 @@
         <v>49</v>
       </c>
       <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
         <v>50</v>
-      </c>
-      <c r="C3" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2794,7 +2792,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2835,7 +2835,14 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>